<commit_message>
Resolve QA errors and rebuild
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-rtlsMessageHeader.xlsx
+++ b/output/StructureDefinition-rtlsMessageHeader.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-06-24T13:15:27-05:00</t>
+    <t>2025-06-24T13:30:24-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3863,7 +3863,7 @@
         <v>88</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>78</v>

</xml_diff>